<commit_message>
Using the new version or RBAC client.
</commit_message>
<xml_diff>
--- a/conf-core/src/main/webapp/resources/import-templates/ccdb_units.xlsx
+++ b/conf-core/src/main/webapp/resources/import-templates/ccdb_units.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="37395" windowHeight="17940"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -19,36 +14,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Copyright</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>OPERATION</t>
+  </si>
+  <si>
+    <t>LGPL3</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>European Spallation Source (ESS)</t>
+  </si>
+  <si>
+    <t>2015/MAY/06</t>
+  </si>
+  <si>
+    <t>Template file to import units in the CCDB</t>
+  </si>
   <si>
     <t>NAME</t>
   </si>
   <si>
-    <t>QUANTITY</t>
+    <t>DESCRIPTION</t>
   </si>
   <si>
     <t>SYMBOL</t>
   </si>
   <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>OPERATION</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Import units file</t>
+    <t>Total names</t>
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>Production</t>
   </si>
 </sst>
 </file>
@@ -81,7 +106,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,28 +138,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,9 +157,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -195,7 +205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,7 +240,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,116 +449,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="9"/>
-    <col min="2" max="5" width="20.7109375" style="8"/>
-    <col min="6" max="16384" width="20.7109375" style="1"/>
+    <col min="1" max="1" width="30.7109375" style="3"/>
+    <col min="4" max="4" width="30.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1">
+        <f xml:space="preserve"> SUMPRODUCT((B9:B65536 &lt;&gt; "") / COUNTIF(B9:B65536, B9:B65536 &amp; ""))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <f xml:space="preserve"> COUNTIF(A8:A65536, "CREATE")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <f xml:space="preserve"> COUNTIF(A8:A65536, "UPDATE")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f xml:space="preserve"> COUNTIF(A8:A65536, "DELETE")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:5" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10">
-        <v>42114</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="E11" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8LQB/jRmrn+HTiYXMV+95QI0JYu/f0YQtbHcT8EHE+HnlfvlR0N0/m4djNcZpX3iLHc7NXGHTqbDpgATZ08AJQ==" saltValue="lSdxEwDQfay9lHmxtgCVkw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <protectedRanges>
-    <protectedRange algorithmName="SHA-512" hashValue="EeGo8NBC4pNhZULZNaKuYvDytr72sNAZGKPQclUfebB9p1K/COIIzmq7ypdmWUrLgKG8YSgznzmYVgZcEd9pmw==" saltValue="ZUQ9+Q/Q4L3Ixt2ynw4A8w==" spinCount="100000" sqref="A1:XFD5" name="Locked header cells"/>
-  </protectedRanges>
-  <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6:A1048576">
-      <formula1>"CREATE,UPDATE,DELETE,END"</formula1>
+  <dataValidations count="4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="B8 C8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="D8"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A1048576">
+      <formula1>"CREATE,UPDATE,DELETE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select one of the possible import operations. If left blank, this line will not be imported. _x000a_This column is not imported into the database; it controls the import process." sqref="A5"/>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid length" error="The unit namer must be between 1 and 32 characters long" sqref="B6:B1048576">
-      <formula1>1</formula1>
-      <formula2>32</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit name (REQUIRED)" prompt="The unique name of the unit" sqref="B5"/>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The symbol text for the unit must be between 1 and 128 characters long." sqref="D6:D1048576">
-      <formula1>1</formula1>
-      <formula2>128</formula2>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid text length" error="The quantity description of the unit must be between 1 and 64 characters long." sqref="C6:C1048576">
-      <formula1>1</formula1>
-      <formula2>64</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Quantity (REQUIRED)" prompt="The quantity this unit describes. E.g.: &quot;length&quot; for unit &quot;meter&quot;." sqref="C5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Symbol (REQUIRED)" prompt="The symbol of the unit. E.g.: &quot;m&quot; for &quot;meter&quot;" sqref="D5"/>
-    <dataValidation type="textLength" allowBlank="1" showErrorMessage="1" errorTitle="Invalid length" error="The length of the description must be between 1 and 255 characters long." prompt="This is the description description." sqref="E6:E1048576">
-      <formula1>1</formula1>
-      <formula2>255</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="E1:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description (REQUIRED)" prompt="The description of the unit for the user." sqref="E5"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="A8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CCDB-216: Updated the code to the new tamplate.
Next : integration tests.
</commit_message>
<xml_diff>
--- a/conf-core/src/main/webapp/resources/import-templates/ccdb_units.xlsx
+++ b/conf-core/src/main/webapp/resources/import-templates/ccdb_units.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="/twiC24/jp4QHQmaIXlVKg6zKK36SE+AZawijxc29Fw0bP4RB6x2m3Z+YsFM16dhOi5Q1YcuA5AwNcQeB6W5kg==" workbookSaltValue="mp3CKO0oFlisoDrQArwULQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -138,16 +144,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,6 +174,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -205,7 +225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,7 +260,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,107 +471,119 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="3"/>
-    <col min="4" max="4" width="30.7109375" style="3"/>
+    <col min="1" max="1" width="30.7109375" style="2"/>
+    <col min="2" max="3" width="30.7109375" style="1"/>
+    <col min="4" max="4" width="30.7109375" style="2"/>
+    <col min="5" max="16384" width="30.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="6">
         <f xml:space="preserve"> SUMPRODUCT((B9:B65536 &lt;&gt; "") / COUNTIF(B9:B65536, B9:B65536 &amp; ""))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="6">
         <f xml:space="preserve"> COUNTIF(A8:A65536, "CREATE")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <f xml:space="preserve"> COUNTIF(A8:A65536, "UPDATE")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <f xml:space="preserve"> COUNTIF(A8:A65536, "DELETE")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:5" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" s="6" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="3"/>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -560,16 +592,18 @@
     </row>
     <row r="11" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="B8 C8"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="D8"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="RoLXS/csV/THvkiknfKGiUT+zKUC3UMEl9NSsD6h+5pju0P/IzyJDUsTHG4XxlmpBQLKh8B+oBbfd2BMXjv88w==" saltValue="EdmBTbBImHOWUBu3R4Tw/w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Description (REQUIRED)" prompt="The description of the unit for the user." sqref="C8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Symbol (REQUIRED)" prompt="The symbol of the unit. E.g.: &quot;m&quot; for &quot;meter&quot;" sqref="D8"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A1048576">
       <formula1>"CREATE,UPDATE,DELETE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Lorem Ipsum" sqref="A8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Select one of the possible import operations. If left blank, this line will not be imported. _x000a_This column is not imported into the database; it controls the import process." sqref="A8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Unit name (REQUIRED)" prompt="The unique name of the unit" sqref="B8"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>